<commit_message>
Adição de Médias no arquivo xlsx
</commit_message>
<xml_diff>
--- a/Teste_1_Jogador_Completo/grupo_duplas.xlsx
+++ b/Teste_1_Jogador_Completo/grupo_duplas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +499,21 @@
           <t>P_Pizza</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>M_Vitorias</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>M_Derrotas</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>M_Empates</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -544,6 +559,15 @@
       <c r="M2" t="n">
         <v>0.2307692307692308</v>
       </c>
+      <c r="N2" t="n">
+        <v>3.384615384615385</v>
+      </c>
+      <c r="O2" t="n">
+        <v>3.307692307692307</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1.230769230769231</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -589,6 +613,15 @@
       <c r="M3" t="n">
         <v>0.2857142857142857</v>
       </c>
+      <c r="N3" t="n">
+        <v>3.571428571428572</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2.857142857142857</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1.285714285714286</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -634,6 +667,15 @@
       <c r="M4" t="n">
         <v>0.1428571428571428</v>
       </c>
+      <c r="N4" t="n">
+        <v>2.428571428571428</v>
+      </c>
+      <c r="O4" t="n">
+        <v>3.428571428571428</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1.714285714285714</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -679,6 +721,15 @@
       <c r="M5" t="n">
         <v>0.1666666666666667</v>
       </c>
+      <c r="N5" t="n">
+        <v>3.333333333333333</v>
+      </c>
+      <c r="O5" t="n">
+        <v>3</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1.666666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -724,6 +775,15 @@
       <c r="M6" t="n">
         <v>0.1666666666666667</v>
       </c>
+      <c r="N6" t="n">
+        <v>2.833333333333333</v>
+      </c>
+      <c r="O6" t="n">
+        <v>2.833333333333333</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1.833333333333333</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -769,6 +829,15 @@
       <c r="M7" t="n">
         <v>0.1666666666666667</v>
       </c>
+      <c r="N7" t="n">
+        <v>3.166666666666667</v>
+      </c>
+      <c r="O7" t="n">
+        <v>2.333333333333333</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1.833333333333333</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -814,6 +883,15 @@
       <c r="M8" t="n">
         <v>0</v>
       </c>
+      <c r="N8" t="n">
+        <v>3.166666666666667</v>
+      </c>
+      <c r="O8" t="n">
+        <v>2</v>
+      </c>
+      <c r="P8" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -859,6 +937,15 @@
       <c r="M9" t="n">
         <v>0.1666666666666667</v>
       </c>
+      <c r="N9" t="n">
+        <v>2.333333333333333</v>
+      </c>
+      <c r="O9" t="n">
+        <v>3</v>
+      </c>
+      <c r="P9" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -904,6 +991,15 @@
       <c r="M10" t="n">
         <v>0.1666666666666667</v>
       </c>
+      <c r="N10" t="n">
+        <v>3.166666666666667</v>
+      </c>
+      <c r="O10" t="n">
+        <v>2.166666666666667</v>
+      </c>
+      <c r="P10" t="n">
+        <v>1.333333333333333</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -949,6 +1045,15 @@
       <c r="M11" t="n">
         <v>0</v>
       </c>
+      <c r="N11" t="n">
+        <v>1.833333333333333</v>
+      </c>
+      <c r="O11" t="n">
+        <v>3.166666666666667</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.8333333333333334</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -994,6 +1099,15 @@
       <c r="M12" t="n">
         <v>0.4</v>
       </c>
+      <c r="N12" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="O12" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="P12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1039,6 +1153,15 @@
       <c r="M13" t="n">
         <v>0.2</v>
       </c>
+      <c r="N13" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="O13" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="P13" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1084,6 +1207,15 @@
       <c r="M14" t="n">
         <v>0</v>
       </c>
+      <c r="N14" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="O14" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="P14" t="n">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1129,6 +1261,15 @@
       <c r="M15" t="n">
         <v>0.5</v>
       </c>
+      <c r="N15" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="O15" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P15" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1174,6 +1315,15 @@
       <c r="M16" t="n">
         <v>0</v>
       </c>
+      <c r="N16" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="O16" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1219,6 +1369,15 @@
       <c r="M17" t="n">
         <v>0.25</v>
       </c>
+      <c r="N17" t="n">
+        <v>3</v>
+      </c>
+      <c r="O17" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="P17" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1264,6 +1423,15 @@
       <c r="M18" t="n">
         <v>0.6666666666666666</v>
       </c>
+      <c r="N18" t="n">
+        <v>5.666666666666667</v>
+      </c>
+      <c r="O18" t="n">
+        <v>2.333333333333333</v>
+      </c>
+      <c r="P18" t="n">
+        <v>1.666666666666667</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1309,6 +1477,15 @@
       <c r="M19" t="n">
         <v>0.3333333333333333</v>
       </c>
+      <c r="N19" t="n">
+        <v>3.333333333333333</v>
+      </c>
+      <c r="O19" t="n">
+        <v>3.333333333333333</v>
+      </c>
+      <c r="P19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1354,6 +1531,15 @@
       <c r="M20" t="n">
         <v>0</v>
       </c>
+      <c r="N20" t="n">
+        <v>3</v>
+      </c>
+      <c r="O20" t="n">
+        <v>2.333333333333333</v>
+      </c>
+      <c r="P20" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1399,6 +1585,15 @@
       <c r="M21" t="n">
         <v>0</v>
       </c>
+      <c r="N21" t="n">
+        <v>1.666666666666667</v>
+      </c>
+      <c r="O21" t="n">
+        <v>3.666666666666667</v>
+      </c>
+      <c r="P21" t="n">
+        <v>1.333333333333333</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1444,6 +1639,15 @@
       <c r="M22" t="n">
         <v>0</v>
       </c>
+      <c r="N22" t="n">
+        <v>1.333333333333333</v>
+      </c>
+      <c r="O22" t="n">
+        <v>2.666666666666667</v>
+      </c>
+      <c r="P22" t="n">
+        <v>1.666666666666667</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1489,6 +1693,15 @@
       <c r="M23" t="n">
         <v>0.5</v>
       </c>
+      <c r="N23" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="O23" t="n">
+        <v>2</v>
+      </c>
+      <c r="P23" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1534,6 +1747,15 @@
       <c r="M24" t="n">
         <v>0.5</v>
       </c>
+      <c r="N24" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="O24" t="n">
+        <v>3</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1579,6 +1801,15 @@
       <c r="M25" t="n">
         <v>0</v>
       </c>
+      <c r="N25" t="n">
+        <v>1</v>
+      </c>
+      <c r="O25" t="n">
+        <v>5</v>
+      </c>
+      <c r="P25" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1624,6 +1855,15 @@
       <c r="M26" t="n">
         <v>0</v>
       </c>
+      <c r="N26" t="n">
+        <v>3</v>
+      </c>
+      <c r="O26" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="P26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1669,6 +1909,15 @@
       <c r="M27" t="n">
         <v>0</v>
       </c>
+      <c r="N27" t="n">
+        <v>3</v>
+      </c>
+      <c r="O27" t="n">
+        <v>4</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1714,6 +1963,15 @@
       <c r="M28" t="n">
         <v>0</v>
       </c>
+      <c r="N28" t="n">
+        <v>3</v>
+      </c>
+      <c r="O28" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P28" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1759,6 +2017,15 @@
       <c r="M29" t="n">
         <v>0.5</v>
       </c>
+      <c r="N29" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="O29" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P29" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1804,6 +2071,15 @@
       <c r="M30" t="n">
         <v>0</v>
       </c>
+      <c r="N30" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="O30" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="P30" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1849,6 +2125,15 @@
       <c r="M31" t="n">
         <v>0</v>
       </c>
+      <c r="N31" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P31" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1894,6 +2179,15 @@
       <c r="M32" t="n">
         <v>0</v>
       </c>
+      <c r="N32" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="O32" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1939,6 +2233,15 @@
       <c r="M33" t="n">
         <v>0</v>
       </c>
+      <c r="N33" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P33" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1984,6 +2287,15 @@
       <c r="M34" t="n">
         <v>0</v>
       </c>
+      <c r="N34" t="n">
+        <v>5</v>
+      </c>
+      <c r="O34" t="n">
+        <v>4</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2029,6 +2341,15 @@
       <c r="M35" t="n">
         <v>1</v>
       </c>
+      <c r="N35" t="n">
+        <v>5</v>
+      </c>
+      <c r="O35" t="n">
+        <v>2</v>
+      </c>
+      <c r="P35" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2074,6 +2395,15 @@
       <c r="M36" t="n">
         <v>0</v>
       </c>
+      <c r="N36" t="n">
+        <v>4</v>
+      </c>
+      <c r="O36" t="n">
+        <v>4</v>
+      </c>
+      <c r="P36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2119,6 +2449,15 @@
       <c r="M37" t="n">
         <v>0</v>
       </c>
+      <c r="N37" t="n">
+        <v>3</v>
+      </c>
+      <c r="O37" t="n">
+        <v>3</v>
+      </c>
+      <c r="P37" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2164,6 +2503,15 @@
       <c r="M38" t="n">
         <v>1</v>
       </c>
+      <c r="N38" t="n">
+        <v>5</v>
+      </c>
+      <c r="O38" t="n">
+        <v>1</v>
+      </c>
+      <c r="P38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2209,6 +2557,15 @@
       <c r="M39" t="n">
         <v>0</v>
       </c>
+      <c r="N39" t="n">
+        <v>3</v>
+      </c>
+      <c r="O39" t="n">
+        <v>3</v>
+      </c>
+      <c r="P39" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2254,6 +2611,15 @@
       <c r="M40" t="n">
         <v>0</v>
       </c>
+      <c r="N40" t="n">
+        <v>3</v>
+      </c>
+      <c r="O40" t="n">
+        <v>3</v>
+      </c>
+      <c r="P40" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2299,6 +2665,15 @@
       <c r="M41" t="n">
         <v>0</v>
       </c>
+      <c r="N41" t="n">
+        <v>2</v>
+      </c>
+      <c r="O41" t="n">
+        <v>4</v>
+      </c>
+      <c r="P41" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2344,6 +2719,15 @@
       <c r="M42" t="n">
         <v>0</v>
       </c>
+      <c r="N42" t="n">
+        <v>2</v>
+      </c>
+      <c r="O42" t="n">
+        <v>4</v>
+      </c>
+      <c r="P42" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2389,6 +2773,15 @@
       <c r="M43" t="n">
         <v>0</v>
       </c>
+      <c r="N43" t="n">
+        <v>1</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0</v>
+      </c>
+      <c r="P43" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2434,6 +2827,15 @@
       <c r="M44" t="n">
         <v>0</v>
       </c>
+      <c r="N44" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" t="n">
+        <v>6</v>
+      </c>
+      <c r="P44" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2479,6 +2881,15 @@
       <c r="M45" t="n">
         <v>0</v>
       </c>
+      <c r="N45" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" t="n">
+        <v>5</v>
+      </c>
+      <c r="P45" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2524,6 +2935,15 @@
       <c r="M46" t="n">
         <v>0</v>
       </c>
+      <c r="N46" t="n">
+        <v>2</v>
+      </c>
+      <c r="O46" t="n">
+        <v>0</v>
+      </c>
+      <c r="P46" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2569,6 +2989,15 @@
       <c r="M47" t="n">
         <v>0</v>
       </c>
+      <c r="N47" t="n">
+        <v>1</v>
+      </c>
+      <c r="O47" t="n">
+        <v>4</v>
+      </c>
+      <c r="P47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2614,6 +3043,15 @@
       <c r="M48" t="n">
         <v>0</v>
       </c>
+      <c r="N48" t="n">
+        <v>1</v>
+      </c>
+      <c r="O48" t="n">
+        <v>4</v>
+      </c>
+      <c r="P48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2659,6 +3097,15 @@
       <c r="M49" t="n">
         <v>0</v>
       </c>
+      <c r="N49" t="n">
+        <v>1</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0</v>
+      </c>
+      <c r="P49" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2702,6 +3149,15 @@
         <v>0.5</v>
       </c>
       <c r="M50" t="n">
+        <v>0</v>
+      </c>
+      <c r="N50" t="n">
+        <v>1</v>
+      </c>
+      <c r="O50" t="n">
+        <v>1</v>
+      </c>
+      <c r="P50" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>